<commit_message>
Corrected how-tos on Forms integrations
</commit_message>
<xml_diff>
--- a/source/_static/files/flow/how-tos/Create-Word-and-XLSX-template.xlsx
+++ b/source/_static/files/flow/how-tos/Create-Word-and-XLSX-template.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="152" documentId="11_924874E5C5FBB6926123EA198B3E8C185103838B" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7BE8A149-BE02-4D05-9EB5-847CEA86BB4B}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aanji\Desktop\documents-docs\source\_static\files\flow\how-tos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24638520-E67C-4E83-BCFD-9CAF9C342376}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5124" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -92,7 +97,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -220,6 +228,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -254,7 +263,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="">
+        <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE9295E0-6D07-46F7-B9F8-1FFBAD7AAA9A}"/>
@@ -287,9 +296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,7 +336,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -433,7 +442,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,65 +595,65 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="21">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -652,7 +661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -660,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -668,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -676,7 +685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -684,7 +693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -692,7 +701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -706,6 +715,7 @@
     <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>